<commit_message>
feat: ran all imports
</commit_message>
<xml_diff>
--- a/import/raw_data/fraunhofer/conversion_efficiency.xlsx
+++ b/import/raw_data/fraunhofer/conversion_efficiency.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bef\GitHub\micat\import\raw_data\fraunhofer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenz/Projekte/micat/import/raw_data/fraunhofer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB73266-2A77-4CB4-BDD9-17D334FD4E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6079252-267A-C948-A175-0EB1E3524381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{0E12F83F-BD87-4A79-86BE-AC2F84F2A603}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="19420" windowHeight="11500" xr2:uid="{0E12F83F-BD87-4A79-86BE-AC2F84F2A603}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>id_primary energy carrier</t>
+    <t>id_final_energy_carrier</t>
   </si>
   <si>
-    <t>id_final_energy_carrier</t>
+    <t>id_primary_energy_carrier</t>
   </si>
 </sst>
 </file>
@@ -88,13 +88,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{C7F9C5BA-ABF6-41E5-9E51-95F0FD9609AD}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -110,7 +109,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -429,17 +428,17 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E15:E16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1">
         <v>2000</v>
@@ -460,17 +459,17 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>0.41</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>0.41</v>
       </c>
       <c r="E2">
@@ -486,17 +485,17 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>0.38</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>0.38</v>
       </c>
       <c r="E3">
@@ -512,17 +511,17 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>0.56999999999999995</v>
       </c>
       <c r="E4">
@@ -538,17 +537,17 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>0.35</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>0.35</v>
       </c>
       <c r="E5">
@@ -564,43 +563,43 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>0.38</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>0.38</v>
       </c>
       <c r="E7">
@@ -616,17 +615,17 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
@@ -642,17 +641,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>0.86</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>0.86</v>
       </c>
       <c r="E9">
@@ -668,17 +667,17 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>0.82</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>0.82</v>
       </c>
       <c r="E10">
@@ -694,17 +693,17 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>6</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>0.89</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>0.89</v>
       </c>
       <c r="E11">
@@ -720,17 +719,17 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>6</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>0.82</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>0.82</v>
       </c>
       <c r="E12">
@@ -746,17 +745,17 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>6</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
@@ -772,43 +771,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>6</v>
       </c>
       <c r="B14">
         <v>6</v>
       </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>6</v>
       </c>
       <c r="B15">
         <v>7</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>2.5</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>2.5</v>
       </c>
       <c r="E15">
@@ -824,7 +823,7 @@
         <v>3.33</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>7</v>
       </c>
@@ -850,7 +849,7 @@
         <v>0.55900000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>7</v>
       </c>
@@ -876,7 +875,7 @@
         <v>0.55900000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -902,7 +901,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>7</v>
       </c>
@@ -928,7 +927,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -954,7 +953,7 @@
         <v>0.66800000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>7</v>
       </c>
@@ -980,7 +979,7 @@
         <v>0.66800000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
feat: working on eurostat import
</commit_message>
<xml_diff>
--- a/import/raw_data/fraunhofer/conversion_efficiency.xlsx
+++ b/import/raw_data/fraunhofer/conversion_efficiency.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bef\GitHub\micat\import\raw_data\fraunhofer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenz/Projekte/micat/import/raw_data/fraunhofer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04869458-877C-4E10-A38B-409EAB497D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3360E4BB-52D5-364C-A5BD-45E272E56172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45984" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{0E12F83F-BD87-4A79-86BE-AC2F84F2A603}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{0E12F83F-BD87-4A79-86BE-AC2F84F2A603}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>id_primary energy carrier</t>
+    <t>id_final_energy_carrier</t>
   </si>
   <si>
-    <t>id_final_energy_carrier</t>
+    <t>id_primary_energy_carrier</t>
   </si>
 </sst>
 </file>
@@ -93,7 +93,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{C7F9C5BA-ABF6-41E5-9E51-95F0FD9609AD}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -428,17 +428,17 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:H15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1">
         <v>2000</v>
@@ -459,7 +459,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -485,7 +485,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -511,7 +511,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -537,7 +537,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -563,7 +563,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -589,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -615,7 +615,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -641,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -667,7 +667,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -693,7 +693,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>6</v>
       </c>
@@ -719,7 +719,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>6</v>
       </c>
@@ -745,7 +745,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>6</v>
       </c>
@@ -771,7 +771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6</v>
       </c>
@@ -797,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>6</v>
       </c>
@@ -823,7 +823,7 @@
         <v>3.33</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>7</v>
       </c>
@@ -849,7 +849,7 @@
         <v>0.55900000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>7</v>
       </c>
@@ -875,7 +875,7 @@
         <v>0.55900000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -901,7 +901,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>7</v>
       </c>
@@ -927,7 +927,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -953,7 +953,7 @@
         <v>0.66800000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>7</v>
       </c>
@@ -979,7 +979,7 @@
         <v>0.66800000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>7</v>
       </c>

</xml_diff>